<commit_message>
new summary and white for playring and using 250 modis
</commit_message>
<xml_diff>
--- a/MasterRawWhitesheets.xlsx
+++ b/MasterRawWhitesheets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10613"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/maxgotts/Desktop/MPALA/Whitesheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9C8038-5492-8743-A312-7B4551479F15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B53BA1CC-D76B-A64B-92B6-B08443078A28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{36B2ED0A-F989-D041-BB6A-DE14AE9EF1AD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7503" uniqueCount="434">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7502" uniqueCount="433">
   <si>
     <t>Date</t>
   </si>
@@ -1215,9 +1215,6 @@
     <t>DSCN4766</t>
   </si>
   <si>
-    <t>`</t>
-  </si>
-  <si>
     <t>Ewaso-Marok River Bank</t>
   </si>
   <si>
@@ -1708,8 +1705,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A334BBC-0BE1-1D4B-AB5E-CA1B598930C6}">
   <dimension ref="A1:AR653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A513" zoomScale="113" workbookViewId="0">
-      <selection activeCell="A544" sqref="A544"/>
+    <sheetView tabSelected="1" topLeftCell="A460" zoomScale="113" workbookViewId="0">
+      <selection activeCell="O477" sqref="O477"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -50484,9 +50481,6 @@
       <c r="N477" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="O477" t="s">
-        <v>393</v>
-      </c>
       <c r="P477" s="1" t="s">
         <v>32</v>
       </c>
@@ -50641,7 +50635,7 @@
         <v>3</v>
       </c>
       <c r="C479" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D479">
         <v>1</v>
@@ -50724,7 +50718,7 @@
         <v>1</v>
       </c>
       <c r="AP479" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AQ479">
         <v>3.3759900000000002E-3</v>
@@ -50738,7 +50732,7 @@
         <v>3</v>
       </c>
       <c r="C480" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D480">
         <v>1</v>
@@ -50845,7 +50839,7 @@
         <v>1</v>
       </c>
       <c r="AP480" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AQ480">
         <v>3.3759900000000002E-3</v>
@@ -50859,7 +50853,7 @@
         <v>3</v>
       </c>
       <c r="C481" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D481">
         <v>2</v>
@@ -50933,7 +50927,7 @@
         <v>3</v>
       </c>
       <c r="AP481" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="AQ481">
         <v>3.3691799999999998E-3</v>
@@ -50947,7 +50941,7 @@
         <v>3</v>
       </c>
       <c r="C482" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D482">
         <v>3</v>
@@ -51032,7 +51026,7 @@
         <v>3</v>
       </c>
       <c r="C483" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D483">
         <v>3</v>
@@ -51067,7 +51061,7 @@
         <v>36.868992981758197</v>
       </c>
       <c r="N483" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P483" s="1" t="s">
         <v>135</v>
@@ -51114,7 +51108,7 @@
         <v>3</v>
       </c>
       <c r="C484" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D484">
         <v>1</v>
@@ -51191,7 +51185,7 @@
         <v>24</v>
       </c>
       <c r="AP484" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AQ484">
         <v>4.5962599999999996E-3</v>
@@ -51205,7 +51199,7 @@
         <v>3</v>
       </c>
       <c r="C485" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D485">
         <v>1</v>
@@ -51282,7 +51276,7 @@
         <v>15</v>
       </c>
       <c r="AP485" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AQ485">
         <v>4.5962599999999996E-3</v>
@@ -51296,7 +51290,7 @@
         <v>3</v>
       </c>
       <c r="C486" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D486">
         <v>2</v>
@@ -51367,7 +51361,7 @@
         <v>50</v>
       </c>
       <c r="AP486" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AQ486">
         <v>3.8689000000000002E-3</v>
@@ -51381,7 +51375,7 @@
         <v>3</v>
       </c>
       <c r="C487" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D487">
         <v>3</v>
@@ -51476,7 +51470,7 @@
         <v>1</v>
       </c>
       <c r="AP487" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="AQ487">
         <v>4.6208500000000001E-3</v>
@@ -51490,7 +51484,7 @@
         <v>3</v>
       </c>
       <c r="C488" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D488">
         <v>1</v>
@@ -51578,7 +51572,7 @@
         <v>3</v>
       </c>
       <c r="C489" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D489">
         <v>2</v>
@@ -51667,7 +51661,7 @@
         <v>3</v>
       </c>
       <c r="C490" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D490">
         <v>3</v>
@@ -51752,7 +51746,7 @@
         <v>3</v>
       </c>
       <c r="C491" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D491">
         <v>1</v>
@@ -51861,7 +51855,7 @@
         <v>3</v>
       </c>
       <c r="C492" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D492">
         <v>2</v>
@@ -51946,7 +51940,7 @@
         <v>3</v>
       </c>
       <c r="C493" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D493">
         <v>2</v>
@@ -52031,7 +52025,7 @@
         <v>4</v>
       </c>
       <c r="C494" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D494">
         <v>1</v>
@@ -52140,7 +52134,7 @@
         <v>4</v>
       </c>
       <c r="C495" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D495">
         <v>2</v>
@@ -52240,7 +52234,7 @@
         <v>4</v>
       </c>
       <c r="C496" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="D496">
         <v>3</v>
@@ -52358,7 +52352,7 @@
         <v>4</v>
       </c>
       <c r="C497" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D497">
         <v>1</v>
@@ -52459,7 +52453,7 @@
         <v>1</v>
       </c>
       <c r="AP497" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AQ497">
         <v>3.5935799999999999E-3</v>
@@ -52473,7 +52467,7 @@
         <v>4</v>
       </c>
       <c r="C498" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D498">
         <v>2</v>
@@ -52547,7 +52541,7 @@
         <v>10</v>
       </c>
       <c r="AP498" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AQ498">
         <v>7.9982000000000002E-4</v>
@@ -52561,7 +52555,7 @@
         <v>4</v>
       </c>
       <c r="C499" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D499">
         <v>3</v>
@@ -52649,7 +52643,7 @@
         <v>4</v>
       </c>
       <c r="C500" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D500">
         <v>1</v>
@@ -52731,7 +52725,7 @@
         <v>4</v>
       </c>
       <c r="C501" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D501">
         <v>2</v>
@@ -52778,7 +52772,7 @@
         <v>34</v>
       </c>
       <c r="S501" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="T501" t="s">
         <v>50</v>
@@ -52816,7 +52810,7 @@
         <v>4</v>
       </c>
       <c r="C502" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D502">
         <v>3</v>
@@ -52898,7 +52892,7 @@
         <v>4</v>
       </c>
       <c r="C503" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D503">
         <v>1</v>
@@ -52945,7 +52939,7 @@
         <v>34</v>
       </c>
       <c r="S503" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="T503" t="s">
         <v>50</v>
@@ -52980,7 +52974,7 @@
         <v>4</v>
       </c>
       <c r="C504" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D504">
         <v>2</v>
@@ -53065,7 +53059,7 @@
         <v>4</v>
       </c>
       <c r="C505" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="D505">
         <v>3</v>
@@ -53150,7 +53144,7 @@
         <v>4</v>
       </c>
       <c r="C506" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D506">
         <v>1</v>
@@ -53224,7 +53218,7 @@
         <v>63</v>
       </c>
       <c r="AP506" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="AQ506">
         <v>1.7064700000000001E-3</v>
@@ -53238,7 +53232,7 @@
         <v>4</v>
       </c>
       <c r="C507" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D507">
         <v>2</v>
@@ -53341,7 +53335,7 @@
         <v>4</v>
       </c>
       <c r="C508" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="D508">
         <v>3</v>
@@ -53450,7 +53444,7 @@
         <v>1</v>
       </c>
       <c r="C509" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D509">
         <v>1</v>
@@ -53547,7 +53541,7 @@
         <v>1</v>
       </c>
       <c r="C510" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D510">
         <v>2</v>
@@ -53612,10 +53606,10 @@
         <v>53</v>
       </c>
       <c r="Y510" t="s">
+        <v>420</v>
+      </c>
+      <c r="Z510" t="s">
         <v>421</v>
-      </c>
-      <c r="Z510" t="s">
-        <v>422</v>
       </c>
       <c r="AA510" t="s">
         <v>63</v>
@@ -53624,7 +53618,7 @@
         <v>200</v>
       </c>
       <c r="AP510" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AQ510">
         <v>2.0838000000000001E-4</v>
@@ -53638,7 +53632,7 @@
         <v>1</v>
       </c>
       <c r="C511" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D511">
         <v>3</v>
@@ -53700,13 +53694,13 @@
         <v>39</v>
       </c>
       <c r="X511" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Y511" t="s">
         <v>41</v>
       </c>
       <c r="Z511" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AA511" t="s">
         <v>63</v>
@@ -53715,7 +53709,7 @@
         <v>170</v>
       </c>
       <c r="AP511" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="AQ511">
         <v>6.4862999999999997E-4</v>
@@ -53729,7 +53723,7 @@
         <v>1</v>
       </c>
       <c r="C512" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D512">
         <v>1</v>
@@ -53794,7 +53788,7 @@
         <v>40</v>
       </c>
       <c r="Y512" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="AA512" t="s">
         <v>63</v>
@@ -53803,7 +53797,7 @@
         <v>120</v>
       </c>
       <c r="AP512" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="AQ512">
         <v>5.7167000000000003E-4</v>
@@ -53817,7 +53811,7 @@
         <v>1</v>
       </c>
       <c r="C513" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D513">
         <v>2</v>
@@ -53879,10 +53873,10 @@
         <v>53</v>
       </c>
       <c r="X513" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Y513" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AA513" t="s">
         <v>63</v>
@@ -53891,7 +53885,7 @@
         <v>100</v>
       </c>
       <c r="AP513" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="AQ513">
         <v>9.0458699999999993E-3</v>
@@ -53905,7 +53899,7 @@
         <v>1</v>
       </c>
       <c r="C514" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="D514">
         <v>3</v>
@@ -53967,13 +53961,13 @@
         <v>53</v>
       </c>
       <c r="X514" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Y514" t="s">
         <v>39</v>
       </c>
       <c r="Z514" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="AA514" t="s">
         <v>43</v>
@@ -53982,7 +53976,7 @@
         <v>250</v>
       </c>
       <c r="AP514" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="AQ514">
         <v>9.3807200000000004E-3</v>
@@ -53996,7 +53990,7 @@
         <v>1</v>
       </c>
       <c r="C515" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D515">
         <v>1</v>
@@ -54058,7 +54052,7 @@
         <v>53</v>
       </c>
       <c r="X515" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="Y515" t="s">
         <v>39</v>
@@ -54070,7 +54064,7 @@
         <v>170</v>
       </c>
       <c r="AP515" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="AQ515">
         <v>2.3100299999999998E-3</v>
@@ -54084,7 +54078,7 @@
         <v>1</v>
       </c>
       <c r="C516" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D516">
         <v>2</v>
@@ -54184,7 +54178,7 @@
         <v>2</v>
       </c>
       <c r="C517" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D517">
         <v>1</v>
@@ -54249,7 +54243,7 @@
         <v>53</v>
       </c>
       <c r="X517" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="Y517" t="s">
         <v>72</v>
@@ -54290,7 +54284,7 @@
         <v>2</v>
       </c>
       <c r="C518" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="D518">
         <v>2</v>
@@ -54352,7 +54346,7 @@
         <v>110</v>
       </c>
       <c r="W518" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="X518" t="s">
         <v>72</v>
@@ -54387,7 +54381,7 @@
         <v>2</v>
       </c>
       <c r="C519" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D519">
         <v>1</v>
@@ -54472,7 +54466,7 @@
         <v>2</v>
       </c>
       <c r="C520" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D520">
         <v>2</v>
@@ -54546,7 +54540,7 @@
         <v>150</v>
       </c>
       <c r="AP520" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="AQ520">
         <v>8.5713E-4</v>
@@ -54560,7 +54554,7 @@
         <v>2</v>
       </c>
       <c r="C521" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="D521">
         <v>3</v>
@@ -54637,7 +54631,7 @@
         <v>110</v>
       </c>
       <c r="AP521" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="AQ521">
         <v>1.0195E-4</v>
@@ -54651,7 +54645,7 @@
         <v>3</v>
       </c>
       <c r="C522" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D522">
         <v>1</v>
@@ -54728,7 +54722,7 @@
         <v>35</v>
       </c>
       <c r="AP522" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ522">
         <v>1.8295099999999999E-3</v>
@@ -54742,7 +54736,7 @@
         <v>3</v>
       </c>
       <c r="C523" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D523">
         <v>1</v>
@@ -54819,7 +54813,7 @@
         <v>70</v>
       </c>
       <c r="AP523" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ523">
         <v>1.8295099999999999E-3</v>
@@ -54833,7 +54827,7 @@
         <v>3</v>
       </c>
       <c r="C524" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D524">
         <v>2</v>
@@ -54910,7 +54904,7 @@
         <v>45</v>
       </c>
       <c r="AP524" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ524">
         <v>3.7491899999999999E-3</v>
@@ -54924,7 +54918,7 @@
         <v>3</v>
       </c>
       <c r="C525" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D525">
         <v>3</v>
@@ -55030,7 +55024,7 @@
         <v>3</v>
       </c>
       <c r="C526" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D526">
         <v>1</v>
@@ -55065,7 +55059,7 @@
         <v>36.867832867406896</v>
       </c>
       <c r="N526" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P526" s="1" t="s">
         <v>135</v>
@@ -55095,7 +55089,7 @@
         <v>90</v>
       </c>
       <c r="Y526" s="1" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="AA526" s="1" t="s">
         <v>43</v>
@@ -55104,7 +55098,7 @@
         <v>5</v>
       </c>
       <c r="AP526" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ526">
         <v>9.8313000000000003E-4</v>
@@ -55118,7 +55112,7 @@
         <v>3</v>
       </c>
       <c r="C527" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D527">
         <v>2</v>
@@ -55153,7 +55147,7 @@
         <v>36.868991616829199</v>
       </c>
       <c r="N527" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="P527" s="1" t="s">
         <v>135</v>
@@ -55195,7 +55189,7 @@
         <v>70</v>
       </c>
       <c r="AP527" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ527">
         <v>2.9032E-4</v>
@@ -55209,7 +55203,7 @@
         <v>3</v>
       </c>
       <c r="C528" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D528">
         <v>2</v>
@@ -55286,7 +55280,7 @@
         <v>10</v>
       </c>
       <c r="AP528" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ528">
         <v>2.9032E-4</v>
@@ -55300,7 +55294,7 @@
         <v>3</v>
       </c>
       <c r="C529" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D529">
         <v>3</v>
@@ -55365,7 +55359,7 @@
         <v>39</v>
       </c>
       <c r="Y529" s="1" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="Z529" s="1" t="s">
         <v>156</v>
@@ -55377,7 +55371,7 @@
         <v>40</v>
       </c>
       <c r="AP529" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ529">
         <v>3.3786200000000001E-3</v>
@@ -55391,7 +55385,7 @@
         <v>4</v>
       </c>
       <c r="C530" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D530">
         <v>1</v>
@@ -55503,7 +55497,7 @@
         <v>4</v>
       </c>
       <c r="C531" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D531">
         <v>2</v>
@@ -55618,7 +55612,7 @@
         <v>4</v>
       </c>
       <c r="C532" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D532">
         <v>3</v>
@@ -55695,7 +55689,7 @@
         <v>26</v>
       </c>
       <c r="AP532" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ532">
         <v>4.9348000000000003E-4</v>
@@ -55709,7 +55703,7 @@
         <v>4</v>
       </c>
       <c r="C533" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D533">
         <v>3</v>
@@ -55786,7 +55780,7 @@
         <v>40</v>
       </c>
       <c r="AP533" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="AQ533">
         <v>4.9348000000000003E-4</v>
@@ -55800,7 +55794,7 @@
         <v>4</v>
       </c>
       <c r="C534" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D534">
         <v>1</v>
@@ -55877,7 +55871,7 @@
         <v>16</v>
       </c>
       <c r="AP534" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ534">
         <v>3.1002600000000001E-3</v>
@@ -55891,7 +55885,7 @@
         <v>4</v>
       </c>
       <c r="C535" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D535">
         <v>2</v>
@@ -56004,7 +55998,7 @@
         <v>4</v>
       </c>
       <c r="C536" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D536">
         <v>2</v>
@@ -56089,7 +56083,7 @@
         <v>4</v>
       </c>
       <c r="C537" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D537">
         <v>3</v>
@@ -56166,7 +56160,7 @@
         <v>18</v>
       </c>
       <c r="AP537" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ537">
         <v>2.2782E-4</v>
@@ -56180,7 +56174,7 @@
         <v>4</v>
       </c>
       <c r="C538" s="6" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D538">
         <v>3</v>
@@ -56268,7 +56262,7 @@
         <v>4</v>
       </c>
       <c r="C539" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D539">
         <v>1</v>
@@ -56356,7 +56350,7 @@
         <v>4</v>
       </c>
       <c r="C540" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D540">
         <v>1</v>
@@ -56433,7 +56427,7 @@
         <v>59</v>
       </c>
       <c r="AP540" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ540">
         <v>4.7889400000000002E-3</v>
@@ -56447,7 +56441,7 @@
         <v>4</v>
       </c>
       <c r="C541" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D541">
         <v>2</v>
@@ -56535,7 +56529,7 @@
         <v>4</v>
       </c>
       <c r="C542" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D542">
         <v>2</v>
@@ -56623,7 +56617,7 @@
         <v>4</v>
       </c>
       <c r="C543" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D543">
         <v>3</v>
@@ -56688,7 +56682,7 @@
         <v>39</v>
       </c>
       <c r="Y543" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Z543" t="s">
         <v>135</v>
@@ -56711,7 +56705,7 @@
         <v>4</v>
       </c>
       <c r="C544" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D544">
         <v>3</v>
@@ -56775,7 +56769,7 @@
         <v>39</v>
       </c>
       <c r="Y544" s="6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="Z544" s="6" t="s">
         <v>135</v>
@@ -56787,7 +56781,7 @@
         <v>150</v>
       </c>
       <c r="AP544" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="AQ544">
         <v>3.9196099999999996E-3</v>

</xml_diff>